<commit_message>
Adaptação do codigo e inclusão de estações
</commit_message>
<xml_diff>
--- a/inputs/config.xlsx
+++ b/inputs/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcio.candido\Documents\GitHub\API-Google-Amazonas\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51E8ABB-58DC-4EE7-B7B2-010F2DAAE39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4971DD80-2442-4C84-96CC-87E976D9B223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13452" yWindow="-16308" windowWidth="29016" windowHeight="16416" tabRatio="508" xr2:uid="{F38AE412-D7AE-4449-939E-ED1C93B8EB71}"/>
+    <workbookView xWindow="-15348" yWindow="-16308" windowWidth="29016" windowHeight="16416" tabRatio="508" activeTab="1" xr2:uid="{F38AE412-D7AE-4449-939E-ED1C93B8EB71}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>codigo</t>
   </si>
@@ -188,9 +188,6 @@
     <t>hybas_6121071910</t>
   </si>
   <si>
-    <t>Óbdos</t>
-  </si>
-  <si>
     <t>hybas_6120251180</t>
   </si>
   <si>
@@ -222,6 +219,15 @@
   </si>
   <si>
     <t>hybas_6120405310</t>
+  </si>
+  <si>
+    <t>Óbidos</t>
+  </si>
+  <si>
+    <t>Fazenda Passarão</t>
+  </si>
+  <si>
+    <t>ANA_14515000</t>
   </si>
 </sst>
 </file>
@@ -773,7 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -816,14 +822,23 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="33" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1181,17 +1196,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7BE1BF-8F74-46EA-A9F3-222E119D5AC4}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="4" width="14.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
@@ -1480,7 +1495,7 @@
         <v>10100000</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>-4.2347000000000001</v>
@@ -1492,7 +1507,7 @@
         <v>45789</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>36</v>
@@ -1519,19 +1534,19 @@
         <v>11400000</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>-3.4569000000000001</v>
       </c>
       <c r="D9">
-        <v>-689119</v>
+        <v>-68.911900000000003</v>
       </c>
       <c r="E9" s="1">
         <v>45789</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>36</v>
@@ -1597,7 +1612,7 @@
         <v>15400000</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <v>-8.7483000000000004</v>
@@ -1609,7 +1624,7 @@
         <v>45789</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>36</v>
@@ -1636,7 +1651,7 @@
         <v>15630000</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12">
         <v>-7.5027999999999997</v>
@@ -1648,7 +1663,7 @@
         <v>45789</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>36</v>
@@ -1714,10 +1729,10 @@
         <v>17050001</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C14">
-        <v>-1.1992</v>
+        <v>-1.9192</v>
       </c>
       <c r="D14">
         <v>-55.513100000000001</v>
@@ -1726,7 +1741,7 @@
         <v>45789</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>36</v>
@@ -1753,7 +1768,7 @@
         <v>17430000</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>-7.3396999999999997</v>
@@ -1765,7 +1780,7 @@
         <v>45789</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>36</v>
@@ -1784,6 +1799,45 @@
         <v>imagens/hybas_6120405310.png</v>
       </c>
       <c r="L15" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14515000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16">
+        <v>3.2078000000000002</v>
+      </c>
+      <c r="D16">
+        <v>-60.571100000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>45789</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" ref="K16" si="2">CONCATENATE("imagens/",F16,".png")</f>
+        <v>imagens/ANA_14515000.png</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1797,17 +1851,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F5CFBB-C983-4FD2-BB58-E31821F9F4DC}">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K131" sqref="K131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="25.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="10.5546875" style="4" customWidth="1"/>
@@ -1819,10 +1873,10 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -3075,10 +3129,10 @@
       <c r="A38" s="15">
         <v>10100000</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="20">
         <v>34700</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="20">
         <v>41085</v>
       </c>
       <c r="D38" s="15">
@@ -3109,10 +3163,10 @@
       <c r="A39" s="15">
         <v>10100000</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="20">
         <v>34700</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="20">
         <v>41085</v>
       </c>
       <c r="D39" s="15">
@@ -3143,10 +3197,10 @@
       <c r="A40" s="15">
         <v>10100000</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="20">
         <v>41086</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="20">
         <v>44561</v>
       </c>
       <c r="D40" s="15">
@@ -3177,10 +3231,10 @@
       <c r="A41" s="15">
         <v>10100000</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="20">
         <v>44562</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="20">
         <v>46022</v>
       </c>
       <c r="D41" s="15">
@@ -3211,10 +3265,10 @@
       <c r="A42" s="4">
         <v>11400000</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="21">
         <v>26846</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="21">
         <v>39710</v>
       </c>
       <c r="D42" s="4">
@@ -3245,10 +3299,10 @@
       <c r="A43" s="4">
         <v>11400000</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="21">
         <v>39711</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="21">
         <v>44561</v>
       </c>
       <c r="D43" s="4">
@@ -3279,10 +3333,10 @@
       <c r="A44" s="4">
         <v>11400000</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="21">
         <v>39711</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="21">
         <v>44561</v>
       </c>
       <c r="D44" s="4">
@@ -3313,10 +3367,10 @@
       <c r="A45" s="4">
         <v>11400000</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="21">
         <v>44562</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="21">
         <v>46022</v>
       </c>
       <c r="D45" s="4">
@@ -3347,10 +3401,10 @@
       <c r="A46" s="15">
         <v>14100000</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="20">
         <v>26299</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="20">
         <v>41909</v>
       </c>
       <c r="D46" s="15">
@@ -3381,10 +3435,10 @@
       <c r="A47" s="15">
         <v>14100000</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="20">
         <v>26299</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="20">
         <v>41909</v>
       </c>
       <c r="D47" s="15">
@@ -3415,10 +3469,10 @@
       <c r="A48" s="15">
         <v>14100000</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="20">
         <v>41910</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="20">
         <v>44561</v>
       </c>
       <c r="D48" s="15">
@@ -3449,10 +3503,10 @@
       <c r="A49" s="15">
         <v>14100000</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="20">
         <v>41910</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="20">
         <v>44561</v>
       </c>
       <c r="D49" s="15">
@@ -3483,10 +3537,10 @@
       <c r="A50" s="15">
         <v>14100000</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="20">
         <v>44364</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="20">
         <v>46022</v>
       </c>
       <c r="D50" s="15">
@@ -3517,10 +3571,10 @@
       <c r="A51" s="15">
         <v>14100000</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="20">
         <v>44364</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="20">
         <v>46022</v>
       </c>
       <c r="D51" s="15">
@@ -3551,10 +3605,10 @@
       <c r="A52" s="4">
         <v>15400000</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="21">
         <v>24563</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="21">
         <v>26181</v>
       </c>
       <c r="D52" s="4">
@@ -3585,10 +3639,10 @@
       <c r="A53" s="4">
         <v>15400000</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="21">
         <v>24563</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="21">
         <v>26181</v>
       </c>
       <c r="D53" s="4">
@@ -3619,10 +3673,10 @@
       <c r="A54" s="4">
         <v>15400000</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="21">
         <v>24563</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="21">
         <v>26181</v>
       </c>
       <c r="D54" s="4">
@@ -3653,10 +3707,10 @@
       <c r="A55" s="4">
         <v>15400000</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="21">
         <v>26182</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="21">
         <v>26766</v>
       </c>
       <c r="D55" s="4">
@@ -3687,10 +3741,10 @@
       <c r="A56" s="4">
         <v>15400000</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="21">
         <v>26182</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56" s="21">
         <v>26766</v>
       </c>
       <c r="D56" s="4">
@@ -3721,10 +3775,10 @@
       <c r="A57" s="4">
         <v>15400000</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" s="21">
         <v>26182</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="21">
         <v>26766</v>
       </c>
       <c r="D57" s="4">
@@ -3755,10 +3809,10 @@
       <c r="A58" s="4">
         <v>15400000</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="21">
         <v>26767</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="21">
         <v>27944</v>
       </c>
       <c r="D58" s="4">
@@ -3789,10 +3843,10 @@
       <c r="A59" s="4">
         <v>15400000</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="21">
         <v>27945</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="21">
         <v>29184</v>
       </c>
       <c r="D59" s="4">
@@ -3823,10 +3877,10 @@
       <c r="A60" s="4">
         <v>15400000</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60" s="21">
         <v>27945</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="21">
         <v>29184</v>
       </c>
       <c r="D60" s="4">
@@ -3857,10 +3911,10 @@
       <c r="A61" s="4">
         <v>15400000</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="21">
         <v>29185</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="21">
         <v>39292</v>
       </c>
       <c r="D61" s="4">
@@ -3891,10 +3945,10 @@
       <c r="A62" s="4">
         <v>15400000</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62" s="21">
         <v>39293</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62" s="21">
         <v>42077</v>
       </c>
       <c r="D62" s="4">
@@ -3925,10 +3979,10 @@
       <c r="A63" s="4">
         <v>15400000</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="21">
         <v>39293</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="21">
         <v>42077</v>
       </c>
       <c r="D63" s="4">
@@ -3959,10 +4013,10 @@
       <c r="A64" s="4">
         <v>15400000</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64" s="21">
         <v>42078</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="21">
         <v>43325</v>
       </c>
       <c r="D64" s="4">
@@ -3993,10 +4047,10 @@
       <c r="A65" s="4">
         <v>15400000</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="21">
         <v>42078</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="21">
         <v>43325</v>
       </c>
       <c r="D65" s="4">
@@ -4027,10 +4081,10 @@
       <c r="A66" s="4">
         <v>15400000</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66" s="21">
         <v>42078</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="21">
         <v>43325</v>
       </c>
       <c r="D66" s="4">
@@ -4061,10 +4115,10 @@
       <c r="A67" s="4">
         <v>15400000</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="21">
         <v>43326</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="21">
         <v>44561</v>
       </c>
       <c r="D67" s="4">
@@ -4095,10 +4149,10 @@
       <c r="A68" s="4">
         <v>15400000</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68" s="21">
         <v>43326</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="21">
         <v>44561</v>
       </c>
       <c r="D68" s="4">
@@ -4129,10 +4183,10 @@
       <c r="A69" s="4">
         <v>15400000</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="21">
         <v>43326</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="21">
         <v>44561</v>
       </c>
       <c r="D69" s="4">
@@ -4163,10 +4217,10 @@
       <c r="A70" s="4">
         <v>15400000</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70" s="21">
         <v>44562</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70" s="21">
         <v>45018</v>
       </c>
       <c r="D70" s="4">
@@ -4197,10 +4251,10 @@
       <c r="A71" s="4">
         <v>15400000</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71" s="21">
         <v>44562</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="21">
         <v>45018</v>
       </c>
       <c r="D71" s="4">
@@ -4231,10 +4285,10 @@
       <c r="A72" s="4">
         <v>15400000</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="21">
         <v>44562</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="21">
         <v>45018</v>
       </c>
       <c r="D72" s="4">
@@ -4265,10 +4319,10 @@
       <c r="A73" s="4">
         <v>15400000</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="21">
         <v>45019</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="21">
         <v>46022</v>
       </c>
       <c r="D73" s="4">
@@ -4299,10 +4353,10 @@
       <c r="A74" s="4">
         <v>15400000</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="21">
         <v>45019</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="21">
         <v>46022</v>
       </c>
       <c r="D74" s="4">
@@ -4333,10 +4387,10 @@
       <c r="A75" s="4">
         <v>15400000</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75" s="21">
         <v>45019</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="21">
         <v>46022</v>
       </c>
       <c r="D75" s="4">
@@ -4367,10 +4421,10 @@
       <c r="A76" s="4">
         <v>15400000</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76" s="21">
         <v>45019</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="21">
         <v>46022</v>
       </c>
       <c r="D76" s="4">
@@ -4401,10 +4455,10 @@
       <c r="A77" s="15">
         <v>15630000</v>
       </c>
-      <c r="B77" s="15">
+      <c r="B77" s="20">
         <v>24580</v>
       </c>
-      <c r="C77" s="15">
+      <c r="C77" s="20">
         <v>33187</v>
       </c>
       <c r="D77" s="15">
@@ -4435,10 +4489,10 @@
       <c r="A78" s="15">
         <v>15630000</v>
       </c>
-      <c r="B78" s="15">
+      <c r="B78" s="20">
         <v>24580</v>
       </c>
-      <c r="C78" s="15">
+      <c r="C78" s="20">
         <v>33187</v>
       </c>
       <c r="D78" s="15">
@@ -4469,10 +4523,10 @@
       <c r="A79" s="15">
         <v>15630000</v>
       </c>
-      <c r="B79" s="15">
+      <c r="B79" s="20">
         <v>24580</v>
       </c>
-      <c r="C79" s="15">
+      <c r="C79" s="20">
         <v>33187</v>
       </c>
       <c r="D79" s="15">
@@ -4503,10 +4557,10 @@
       <c r="A80" s="15">
         <v>15630000</v>
       </c>
-      <c r="B80" s="15">
+      <c r="B80" s="20">
         <v>33188</v>
       </c>
-      <c r="C80" s="15">
+      <c r="C80" s="20">
         <v>41941</v>
       </c>
       <c r="D80" s="15">
@@ -4537,10 +4591,10 @@
       <c r="A81" s="15">
         <v>15630000</v>
       </c>
-      <c r="B81" s="15">
+      <c r="B81" s="20">
         <v>33188</v>
       </c>
-      <c r="C81" s="15">
+      <c r="C81" s="20">
         <v>41941</v>
       </c>
       <c r="D81" s="15">
@@ -4571,10 +4625,10 @@
       <c r="A82" s="15">
         <v>15630000</v>
       </c>
-      <c r="B82" s="15">
+      <c r="B82" s="20">
         <v>41942</v>
       </c>
-      <c r="C82" s="15">
+      <c r="C82" s="20">
         <v>44561</v>
       </c>
       <c r="D82" s="15">
@@ -4605,10 +4659,10 @@
       <c r="A83" s="15">
         <v>15630000</v>
       </c>
-      <c r="B83" s="15">
+      <c r="B83" s="20">
         <v>41942</v>
       </c>
-      <c r="C83" s="15">
+      <c r="C83" s="20">
         <v>44561</v>
       </c>
       <c r="D83" s="15">
@@ -4639,10 +4693,10 @@
       <c r="A84" s="15">
         <v>15630000</v>
       </c>
-      <c r="B84" s="15">
+      <c r="B84" s="20">
         <v>41942</v>
       </c>
-      <c r="C84" s="15">
+      <c r="C84" s="20">
         <v>44561</v>
       </c>
       <c r="D84" s="15">
@@ -4673,10 +4727,10 @@
       <c r="A85" s="15">
         <v>15630000</v>
       </c>
-      <c r="B85" s="15">
+      <c r="B85" s="20">
         <v>44562</v>
       </c>
-      <c r="C85" s="15">
+      <c r="C85" s="20">
         <v>46022</v>
       </c>
       <c r="D85" s="15">
@@ -4707,10 +4761,10 @@
       <c r="A86" s="15">
         <v>15630000</v>
       </c>
-      <c r="B86" s="15">
+      <c r="B86" s="20">
         <v>44562</v>
       </c>
-      <c r="C86" s="15">
+      <c r="C86" s="20">
         <v>46022</v>
       </c>
       <c r="D86" s="15">
@@ -4741,10 +4795,10 @@
       <c r="A87" s="15">
         <v>15630000</v>
       </c>
-      <c r="B87" s="15">
+      <c r="B87" s="20">
         <v>44562</v>
       </c>
-      <c r="C87" s="15">
+      <c r="C87" s="20">
         <v>46022</v>
       </c>
       <c r="D87" s="15">
@@ -4775,10 +4829,10 @@
       <c r="A88" s="4">
         <v>16030000</v>
       </c>
-      <c r="B88" s="4">
+      <c r="B88" s="21">
         <v>39508</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88" s="21">
         <v>42364</v>
       </c>
       <c r="D88" s="4">
@@ -4809,10 +4863,10 @@
       <c r="A89" s="4">
         <v>16030000</v>
       </c>
-      <c r="B89" s="4">
+      <c r="B89" s="21">
         <v>39508</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="21">
         <v>42364</v>
       </c>
       <c r="D89" s="4">
@@ -4843,10 +4897,10 @@
       <c r="A90" s="4">
         <v>16030000</v>
       </c>
-      <c r="B90" s="4">
+      <c r="B90" s="21">
         <v>42365</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="21">
         <v>44561</v>
       </c>
       <c r="D90" s="4">
@@ -4877,10 +4931,10 @@
       <c r="A91" s="4">
         <v>16030000</v>
       </c>
-      <c r="B91" s="4">
+      <c r="B91" s="21">
         <v>44562</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91" s="21">
         <v>46022</v>
       </c>
       <c r="D91" s="4">
@@ -4911,10 +4965,10 @@
       <c r="A92" s="15">
         <v>17050001</v>
       </c>
-      <c r="B92" s="15">
+      <c r="B92" s="20">
         <v>24869</v>
       </c>
-      <c r="C92" s="15">
+      <c r="C92" s="20">
         <v>44561</v>
       </c>
       <c r="D92" s="15">
@@ -4945,10 +4999,10 @@
       <c r="A93" s="15">
         <v>17050001</v>
       </c>
-      <c r="B93" s="15">
+      <c r="B93" s="20">
         <v>24869</v>
       </c>
-      <c r="C93" s="15">
+      <c r="C93" s="20">
         <v>44561</v>
       </c>
       <c r="D93" s="15">
@@ -4979,10 +5033,10 @@
       <c r="A94" s="15">
         <v>17050001</v>
       </c>
-      <c r="B94" s="15">
+      <c r="B94" s="20">
         <v>44562</v>
       </c>
-      <c r="C94" s="15">
+      <c r="C94" s="20">
         <v>46022</v>
       </c>
       <c r="D94" s="15">
@@ -5013,10 +5067,10 @@
       <c r="A95" s="15">
         <v>17050001</v>
       </c>
-      <c r="B95" s="15">
+      <c r="B95" s="20">
         <v>44562</v>
       </c>
-      <c r="C95" s="15">
+      <c r="C95" s="20">
         <v>46022</v>
       </c>
       <c r="D95" s="15">
@@ -5047,10 +5101,10 @@
       <c r="A96" s="15">
         <v>17050001</v>
       </c>
-      <c r="B96" s="15">
+      <c r="B96" s="20">
         <v>44562</v>
       </c>
-      <c r="C96" s="15">
+      <c r="C96" s="20">
         <v>46022</v>
       </c>
       <c r="D96" s="15">
@@ -5081,10 +5135,10 @@
       <c r="A97" s="4">
         <v>17430000</v>
       </c>
-      <c r="B97" s="4">
+      <c r="B97" s="21">
         <v>27699</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="21">
         <v>31374</v>
       </c>
       <c r="D97" s="4">
@@ -5115,10 +5169,10 @@
       <c r="A98" s="4">
         <v>17430000</v>
       </c>
-      <c r="B98" s="4">
+      <c r="B98" s="21">
         <v>27699</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98" s="21">
         <v>31374</v>
       </c>
       <c r="D98" s="4">
@@ -5149,10 +5203,10 @@
       <c r="A99" s="4">
         <v>17430000</v>
       </c>
-      <c r="B99" s="4">
+      <c r="B99" s="21">
         <v>31375</v>
       </c>
-      <c r="C99" s="4">
+      <c r="C99" s="21">
         <v>32979</v>
       </c>
       <c r="D99" s="4">
@@ -5183,10 +5237,10 @@
       <c r="A100" s="4">
         <v>17430000</v>
       </c>
-      <c r="B100" s="4">
+      <c r="B100" s="21">
         <v>31375</v>
       </c>
-      <c r="C100" s="4">
+      <c r="C100" s="21">
         <v>32979</v>
       </c>
       <c r="D100" s="4">
@@ -5217,10 +5271,10 @@
       <c r="A101" s="4">
         <v>17430000</v>
       </c>
-      <c r="B101" s="4">
+      <c r="B101" s="21">
         <v>31375</v>
       </c>
-      <c r="C101" s="4">
+      <c r="C101" s="21">
         <v>32979</v>
       </c>
       <c r="D101" s="4">
@@ -5251,10 +5305,10 @@
       <c r="A102" s="4">
         <v>17430000</v>
       </c>
-      <c r="B102" s="4">
+      <c r="B102" s="21">
         <v>34182</v>
       </c>
-      <c r="C102" s="4">
+      <c r="C102" s="21">
         <v>38046</v>
       </c>
       <c r="D102" s="4">
@@ -5285,10 +5339,10 @@
       <c r="A103" s="4">
         <v>17430000</v>
       </c>
-      <c r="B103" s="4">
+      <c r="B103" s="21">
         <v>34182</v>
       </c>
-      <c r="C103" s="4">
+      <c r="C103" s="21">
         <v>38046</v>
       </c>
       <c r="D103" s="4">
@@ -5319,10 +5373,10 @@
       <c r="A104" s="4">
         <v>17430000</v>
       </c>
-      <c r="B104" s="4">
+      <c r="B104" s="21">
         <v>34182</v>
       </c>
-      <c r="C104" s="4">
+      <c r="C104" s="21">
         <v>38046</v>
       </c>
       <c r="D104" s="4">
@@ -5353,10 +5407,10 @@
       <c r="A105" s="4">
         <v>17430000</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B105" s="21">
         <v>38047</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C105" s="21">
         <v>40478</v>
       </c>
       <c r="D105" s="4">
@@ -5387,10 +5441,10 @@
       <c r="A106" s="4">
         <v>17430000</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B106" s="21">
         <v>38047</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C106" s="21">
         <v>40478</v>
       </c>
       <c r="D106" s="4">
@@ -5421,10 +5475,10 @@
       <c r="A107" s="4">
         <v>17430000</v>
       </c>
-      <c r="B107" s="4">
+      <c r="B107" s="21">
         <v>40479</v>
       </c>
-      <c r="C107" s="4">
+      <c r="C107" s="21">
         <v>42031</v>
       </c>
       <c r="D107" s="4">
@@ -5455,10 +5509,10 @@
       <c r="A108" s="4">
         <v>17430000</v>
       </c>
-      <c r="B108" s="4">
+      <c r="B108" s="21">
         <v>40479</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C108" s="21">
         <v>42031</v>
       </c>
       <c r="D108" s="4">
@@ -5489,10 +5543,10 @@
       <c r="A109" s="4">
         <v>17430000</v>
       </c>
-      <c r="B109" s="4">
+      <c r="B109" s="21">
         <v>42032</v>
       </c>
-      <c r="C109" s="4">
+      <c r="C109" s="21">
         <v>44561</v>
       </c>
       <c r="D109" s="4">
@@ -5523,10 +5577,10 @@
       <c r="A110" s="4">
         <v>17430000</v>
       </c>
-      <c r="B110" s="4">
+      <c r="B110" s="21">
         <v>42032</v>
       </c>
-      <c r="C110" s="4">
+      <c r="C110" s="21">
         <v>44561</v>
       </c>
       <c r="D110" s="4">
@@ -5557,10 +5611,10 @@
       <c r="A111" s="4">
         <v>17430000</v>
       </c>
-      <c r="B111" s="4">
+      <c r="B111" s="21">
         <v>42032</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C111" s="21">
         <v>44561</v>
       </c>
       <c r="D111" s="4">
@@ -5591,10 +5645,10 @@
       <c r="A112" s="4">
         <v>17430000</v>
       </c>
-      <c r="B112" s="4">
+      <c r="B112" s="21">
         <v>44562</v>
       </c>
-      <c r="C112" s="4">
+      <c r="C112" s="21">
         <v>46022</v>
       </c>
       <c r="D112" s="4">
@@ -5625,10 +5679,10 @@
       <c r="A113" s="4">
         <v>17430000</v>
       </c>
-      <c r="B113" s="4">
+      <c r="B113" s="21">
         <v>44562</v>
       </c>
-      <c r="C113" s="4">
+      <c r="C113" s="21">
         <v>46022</v>
       </c>
       <c r="D113" s="4">
@@ -5659,10 +5713,10 @@
       <c r="A114" s="4">
         <v>17430000</v>
       </c>
-      <c r="B114" s="4">
+      <c r="B114" s="21">
         <v>44562</v>
       </c>
-      <c r="C114" s="4">
+      <c r="C114" s="21">
         <v>46022</v>
       </c>
       <c r="D114" s="4">
@@ -5687,6 +5741,380 @@
       <c r="J114" s="16">
         <f t="shared" si="5"/>
         <v>29632.628182193966</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B115" s="20">
+        <v>28246</v>
+      </c>
+      <c r="C115" s="20">
+        <v>37447</v>
+      </c>
+      <c r="D115" s="15">
+        <v>470</v>
+      </c>
+      <c r="E115" s="15">
+        <v>743</v>
+      </c>
+      <c r="F115" s="15">
+        <v>277.97280000000001</v>
+      </c>
+      <c r="G115" s="15">
+        <v>4.38</v>
+      </c>
+      <c r="H115" s="15">
+        <v>1.387</v>
+      </c>
+      <c r="I115" s="11">
+        <f t="shared" ref="I115:I125" si="6">$F115*(D115/100-$G115)^$H115</f>
+        <v>57.232843255534014</v>
+      </c>
+      <c r="J115" s="11">
+        <f t="shared" ref="J115:J125" si="7">$F115*(E115/100-$G115)^$H115</f>
+        <v>1305.3476116485551</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B116" s="20">
+        <v>28246</v>
+      </c>
+      <c r="C116" s="20">
+        <v>37447</v>
+      </c>
+      <c r="D116" s="15">
+        <v>743</v>
+      </c>
+      <c r="E116" s="15">
+        <v>1117</v>
+      </c>
+      <c r="F116" s="15">
+        <v>249.72730000000001</v>
+      </c>
+      <c r="G116" s="15">
+        <v>4.38</v>
+      </c>
+      <c r="H116" s="15">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="I116" s="11">
+        <f t="shared" si="6"/>
+        <v>1305.2168850590349</v>
+      </c>
+      <c r="J116" s="11">
+        <f t="shared" si="7"/>
+        <v>4276.898040226607</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B117" s="20">
+        <v>28246</v>
+      </c>
+      <c r="C117" s="20">
+        <v>37447</v>
+      </c>
+      <c r="D117" s="15">
+        <v>1117</v>
+      </c>
+      <c r="E117" s="15">
+        <v>1300</v>
+      </c>
+      <c r="F117" s="15">
+        <v>203.11070000000001</v>
+      </c>
+      <c r="G117" s="15">
+        <v>4.83</v>
+      </c>
+      <c r="H117" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="I117" s="11">
+        <f t="shared" si="6"/>
+        <v>4277.4021010390343</v>
+      </c>
+      <c r="J117" s="11">
+        <f t="shared" si="7"/>
+        <v>6499.7880667998752</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B118" s="20">
+        <v>37448</v>
+      </c>
+      <c r="C118" s="20">
+        <v>42453</v>
+      </c>
+      <c r="D118" s="15">
+        <v>460</v>
+      </c>
+      <c r="E118" s="15">
+        <v>778</v>
+      </c>
+      <c r="F118" s="15">
+        <v>249.72730000000001</v>
+      </c>
+      <c r="G118" s="15">
+        <v>4.25</v>
+      </c>
+      <c r="H118" s="15">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="I118" s="11">
+        <f t="shared" si="6"/>
+        <v>52.640369789841998</v>
+      </c>
+      <c r="J118" s="11">
+        <f t="shared" si="7"/>
+        <v>1621.1227846738614</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B119" s="20">
+        <v>37448</v>
+      </c>
+      <c r="C119" s="20">
+        <v>42453</v>
+      </c>
+      <c r="D119" s="15">
+        <v>778</v>
+      </c>
+      <c r="E119" s="15">
+        <v>1300</v>
+      </c>
+      <c r="F119" s="15">
+        <v>203.11070000000001</v>
+      </c>
+      <c r="G119" s="15">
+        <v>4.12</v>
+      </c>
+      <c r="H119" s="15">
+        <v>1.601</v>
+      </c>
+      <c r="I119" s="11">
+        <f t="shared" si="6"/>
+        <v>1621.3098479008493</v>
+      </c>
+      <c r="J119" s="11">
+        <f t="shared" si="7"/>
+        <v>6701.0361546472359</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B120" s="20">
+        <v>42454</v>
+      </c>
+      <c r="C120" s="20">
+        <v>44561</v>
+      </c>
+      <c r="D120" s="15">
+        <v>460</v>
+      </c>
+      <c r="E120" s="15">
+        <v>1070</v>
+      </c>
+      <c r="F120" s="15">
+        <v>262.9742</v>
+      </c>
+      <c r="G120" s="15">
+        <v>4.34</v>
+      </c>
+      <c r="H120" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="I120" s="11">
+        <f t="shared" si="6"/>
+        <v>37.292757502204466</v>
+      </c>
+      <c r="J120" s="11">
+        <f t="shared" si="7"/>
+        <v>3845.2622138214247</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B121" s="20">
+        <v>42454</v>
+      </c>
+      <c r="C121" s="20">
+        <v>44561</v>
+      </c>
+      <c r="D121" s="15">
+        <v>1070</v>
+      </c>
+      <c r="E121" s="15">
+        <v>1117</v>
+      </c>
+      <c r="F121" s="15">
+        <v>249.72730000000001</v>
+      </c>
+      <c r="G121" s="15">
+        <v>4.38</v>
+      </c>
+      <c r="H121" s="15">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="I121" s="11">
+        <f t="shared" si="6"/>
+        <v>3845.2931011661321</v>
+      </c>
+      <c r="J121" s="11">
+        <f t="shared" si="7"/>
+        <v>4276.898040226607</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B122" s="20">
+        <v>42454</v>
+      </c>
+      <c r="C122" s="20">
+        <v>44561</v>
+      </c>
+      <c r="D122" s="15">
+        <v>1117</v>
+      </c>
+      <c r="E122" s="15">
+        <v>1300</v>
+      </c>
+      <c r="F122" s="15">
+        <v>203.11070000000001</v>
+      </c>
+      <c r="G122" s="15">
+        <v>4.83</v>
+      </c>
+      <c r="H122" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="I122" s="11">
+        <f t="shared" si="6"/>
+        <v>4277.4021010390343</v>
+      </c>
+      <c r="J122" s="11">
+        <f t="shared" si="7"/>
+        <v>6499.7880667998752</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B123" s="20">
+        <v>44562</v>
+      </c>
+      <c r="C123" s="20">
+        <v>46022</v>
+      </c>
+      <c r="D123" s="15">
+        <v>460</v>
+      </c>
+      <c r="E123" s="15">
+        <v>1070</v>
+      </c>
+      <c r="F123" s="15">
+        <v>262.9742</v>
+      </c>
+      <c r="G123" s="15">
+        <v>4.34</v>
+      </c>
+      <c r="H123" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="I123" s="11">
+        <f t="shared" si="6"/>
+        <v>37.292757502204466</v>
+      </c>
+      <c r="J123" s="11">
+        <f t="shared" si="7"/>
+        <v>3845.2622138214247</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B124" s="20">
+        <v>44562</v>
+      </c>
+      <c r="C124" s="20">
+        <v>46022</v>
+      </c>
+      <c r="D124" s="15">
+        <v>1070</v>
+      </c>
+      <c r="E124" s="15">
+        <v>1117</v>
+      </c>
+      <c r="F124" s="15">
+        <v>249.72730000000001</v>
+      </c>
+      <c r="G124" s="15">
+        <v>4.38</v>
+      </c>
+      <c r="H124" s="15">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="I124" s="11">
+        <f t="shared" si="6"/>
+        <v>3845.2931011661321</v>
+      </c>
+      <c r="J124" s="11">
+        <f t="shared" si="7"/>
+        <v>4276.898040226607</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="15">
+        <v>14515000</v>
+      </c>
+      <c r="B125" s="20">
+        <v>44562</v>
+      </c>
+      <c r="C125" s="20">
+        <v>46022</v>
+      </c>
+      <c r="D125" s="15">
+        <v>1117</v>
+      </c>
+      <c r="E125" s="15">
+        <v>1300</v>
+      </c>
+      <c r="F125" s="15">
+        <v>203.11070000000001</v>
+      </c>
+      <c r="G125" s="15">
+        <v>4.83</v>
+      </c>
+      <c r="H125" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="I125" s="11">
+        <f t="shared" si="6"/>
+        <v>4277.4021010390343</v>
+      </c>
+      <c r="J125" s="11">
+        <f t="shared" si="7"/>
+        <v>6499.7880667998752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>